<commit_message>
Fixed failed tests in 1PContainer due to changed response parameters related to saved search
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProjectContainerTest.xlsx
+++ b/src/test/test-data/ProjectContainerTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Project - Owner" sheetId="1" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>?itemType=all</t>
   </si>
   <si>
-    <t>status=200||contents.patents=0||contents.wos=0||contents.posts=0||contents.documents=0||contents.dra_ss=0||contents.total=0</t>
-  </si>
-  <si>
     <t>{ "ispublic": true }</t>
   </si>
   <si>
@@ -652,9 +649,6 @@
     <t>{"documents":[{"name":"Updated GD name","parent":"container","parentId":"(OPQA-4043_id)","parentType":"document","id":"0B175X3HOM71HN0VDMXpiOW5CVVU","url":"https://drive.google.com/file/d/0B175X3HOM71HcXZkby1qNkFXWFE/view?usp=drive_web"}]}</t>
   </si>
   <si>
-    <t>status=200||id=(OPQA-4043_id)||type=project||userid=(SYS_USER1)||ispublic=false||contents.patents=2||contents.wos=2||contents.posts=2||contents.documents=3||contents.dra_ss=0||contents.total=9</t>
-  </si>
-  <si>
     <t>/container/(OPQA-4043_id)/items?itemType=wos&amp;sortoption=latestupdated</t>
   </si>
   <si>
@@ -694,9 +688,6 @@
     <t>status=200||public_count=1||private_count=0||total_count=1||public[0].id=(OPQA-4043_1_id)</t>
   </si>
   <si>
-    <t>status=200||id=(OPQA-4043_1_id)||type=project||userid=(SYS_USER1)||ispublic=true||contents.patents=2||contents.wos=2||contents.posts=2||contents.documents=1||contents.dra_ss=0||contents.total=7</t>
-  </si>
-  <si>
     <t>/container/(OPQA-4043_1_id)/items/(OPQA-896_hits.hits[0]._id)</t>
   </si>
   <si>
@@ -1037,6 +1028,15 @@
   </si>
   <si>
     <t>/invites/delete/(OPQA-4089_inviteResponses[1].inviteId)</t>
+  </si>
+  <si>
+    <t>status=200||contents.patents=0||contents.wos=0||contents.posts=0||contents.documents=0||contents.sse=0||contents.dra_td_sse=0||contents.ipa_sse=0||contents.total=0</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4043_id)||type=project||userid=(SYS_USER1)||ispublic=false||contents.patents=2||contents.wos=2||contents.posts=2||contents.documents=3||contents.sse=0||contents.dra_td_sse=0||contents.ipa_sse=0||contents.total=9</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-4043_1_id)||type=project||userid=(SYS_USER1)||ispublic=true||contents.patents=2||contents.wos=2||contents.posts=2||contents.documents=1||contents.sse=0||contents.dra_td_sse=0||contents.ipa_sse=0||contents.total=7</t>
   </si>
 </sst>
 </file>
@@ -1455,7 +1455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L51"/>
     </sheetView>
   </sheetViews>
@@ -1539,7 +1539,7 @@
         <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L2"/>
     </row>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="F3"/>
       <c r="G3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3"/>
@@ -1569,7 +1569,7 @@
         <v>14</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L3"/>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="F4"/>
       <c r="G4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4"/>
@@ -1599,7 +1599,7 @@
         <v>14</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L4"/>
     </row>
@@ -1635,10 +1635,10 @@
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="47.25">
       <c r="A6" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>36</v>
@@ -1653,7 +1653,7 @@
         <v>26</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6"/>
@@ -1665,10 +1665,10 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="360">
       <c r="A7" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>36</v>
@@ -1684,11 +1684,11 @@
       </c>
       <c r="G7"/>
       <c r="H7" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7"/>
       <c r="J7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>38</v>
@@ -1697,10 +1697,10 @@
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="105">
       <c r="A8" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>36</v>
@@ -1716,11 +1716,11 @@
       </c>
       <c r="G8"/>
       <c r="H8" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8"/>
       <c r="J8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>38</v>
@@ -1729,16 +1729,16 @@
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="300">
       <c r="A9" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>25</v>
@@ -1748,29 +1748,29 @@
       </c>
       <c r="G9"/>
       <c r="H9" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="105">
       <c r="A10" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>25</v>
@@ -1780,61 +1780,61 @@
       </c>
       <c r="G10"/>
       <c r="H10" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A11" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11"/>
       <c r="H11" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11"/>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="375">
       <c r="A12" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>25</v>
@@ -1844,29 +1844,29 @@
       </c>
       <c r="G12"/>
       <c r="H12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12"/>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="375">
       <c r="A13" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>25</v>
@@ -1876,29 +1876,29 @@
       </c>
       <c r="G13"/>
       <c r="H13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="75">
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A14" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>1</v>
@@ -1911,26 +1911,26 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>42</v>
+        <v>337</v>
       </c>
       <c r="K14"/>
       <c r="L14"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="30">
       <c r="A15" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>1</v>
@@ -1941,26 +1941,26 @@
       <c r="G15"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A16" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>25</v>
@@ -1970,25 +1970,25 @@
       </c>
       <c r="G16"/>
       <c r="H16" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L16"/>
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1" ht="47.25">
       <c r="A17" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>36</v>
@@ -2003,30 +2003,30 @@
         <v>26</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17"/>
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1" ht="75">
       <c r="A18" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>23</v>
@@ -2035,32 +2035,32 @@
         <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18"/>
     </row>
     <row r="19" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A19" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>23</v>
@@ -2069,66 +2069,66 @@
         <v>24</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19"/>
     </row>
     <row r="20" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A20" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20"/>
     </row>
     <row r="21" spans="1:12" s="1" customFormat="1" ht="75">
       <c r="A21" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>23</v>
@@ -2137,32 +2137,32 @@
         <v>24</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12" s="1" customFormat="1" ht="105">
       <c r="A22" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>23</v>
@@ -2171,32 +2171,32 @@
         <v>24</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K22"/>
       <c r="L22"/>
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1" ht="105">
       <c r="A23" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>23</v>
@@ -2205,32 +2205,32 @@
         <v>24</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K23"/>
       <c r="L23"/>
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" ht="375">
       <c r="A24" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>23</v>
@@ -2239,32 +2239,32 @@
         <v>24</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K24"/>
       <c r="L24"/>
     </row>
     <row r="25" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A25" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>23</v>
@@ -2274,29 +2274,29 @@
       </c>
       <c r="G25"/>
       <c r="H25" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K25"/>
       <c r="L25"/>
     </row>
     <row r="26" spans="1:12" s="1" customFormat="1" ht="180">
       <c r="A26" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>23</v>
@@ -2306,29 +2306,29 @@
       </c>
       <c r="G26"/>
       <c r="H26" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K26"/>
       <c r="L26"/>
     </row>
     <row r="27" spans="1:12" s="1" customFormat="1" ht="120">
       <c r="A27" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>1</v>
@@ -2337,30 +2337,30 @@
         <v>26</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K27"/>
       <c r="L27"/>
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" ht="105">
       <c r="A28" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>23</v>
@@ -2370,61 +2370,61 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K28"/>
       <c r="L28"/>
     </row>
     <row r="29" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A29" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G29"/>
       <c r="H29" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K29"/>
       <c r="L29"/>
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A30" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>25</v>
@@ -2434,29 +2434,29 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K30"/>
       <c r="L30"/>
     </row>
     <row r="31" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A31" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>23</v>
@@ -2466,29 +2466,29 @@
       </c>
       <c r="G31"/>
       <c r="H31" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K31"/>
       <c r="L31"/>
     </row>
     <row r="32" spans="1:12" s="1" customFormat="1" ht="180">
       <c r="A32" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>23</v>
@@ -2498,29 +2498,29 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K32"/>
       <c r="L32"/>
     </row>
     <row r="33" spans="1:12" s="1" customFormat="1" ht="120">
       <c r="A33" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>23</v>
@@ -2530,29 +2530,29 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K33"/>
       <c r="L33"/>
     </row>
     <row r="34" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A34" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>25</v>
@@ -2562,29 +2562,29 @@
       </c>
       <c r="G34"/>
       <c r="H34" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K34"/>
       <c r="L34"/>
     </row>
     <row r="35" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A35" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>1</v>
@@ -2593,24 +2593,24 @@
         <v>26</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="K35" s="7"/>
       <c r="L35"/>
     </row>
     <row r="36" spans="1:12" s="1" customFormat="1" ht="75">
       <c r="A36" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>36</v>
@@ -2625,30 +2625,30 @@
         <v>26</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="K36"/>
       <c r="L36"/>
     </row>
-    <row r="37" spans="1:12" s="1" customFormat="1" ht="105">
+    <row r="37" spans="1:12" s="1" customFormat="1" ht="120">
       <c r="A37" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>1</v>
@@ -2659,26 +2659,26 @@
       <c r="G37"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>211</v>
+        <v>338</v>
       </c>
       <c r="K37"/>
       <c r="L37"/>
     </row>
     <row r="38" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A38" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>1</v>
@@ -2687,26 +2687,26 @@
       <c r="G38"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K38"/>
       <c r="L38"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A39" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>1</v>
@@ -2715,26 +2715,26 @@
       <c r="G39"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K39"/>
       <c r="L39"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="195">
       <c r="A40" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>1</v>
@@ -2747,26 +2747,26 @@
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K40"/>
       <c r="L40"/>
     </row>
     <row r="41" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A41" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>1</v>
@@ -2779,26 +2779,26 @@
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K41"/>
       <c r="L41"/>
     </row>
     <row r="42" spans="1:12" s="1" customFormat="1" ht="75">
       <c r="A42" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>1</v>
@@ -2807,30 +2807,30 @@
         <v>26</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="K42"/>
       <c r="L42"/>
     </row>
     <row r="43" spans="1:12" s="1" customFormat="1" ht="30">
       <c r="A43" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>27</v>
@@ -2843,58 +2843,58 @@
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K43"/>
       <c r="L43"/>
     </row>
     <row r="44" spans="1:12" s="1" customFormat="1" ht="45">
       <c r="A44" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K44"/>
       <c r="L44"/>
     </row>
     <row r="45" spans="1:12" s="1" customFormat="1" ht="30">
       <c r="A45" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>27</v>
@@ -2907,26 +2907,26 @@
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K45"/>
       <c r="L45"/>
     </row>
     <row r="46" spans="1:12" ht="75">
       <c r="A46" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>23</v>
@@ -2935,31 +2935,31 @@
         <v>24</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:12" ht="75">
       <c r="A47" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>23</v>
@@ -2968,31 +2968,31 @@
         <v>24</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:12" ht="30">
       <c r="A48" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>27</v>
@@ -3003,7 +3003,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>14</v>
@@ -3012,45 +3012,45 @@
     </row>
     <row r="49" spans="1:11" ht="45">
       <c r="A49" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K49" s="1"/>
     </row>
     <row r="50" spans="1:11" ht="30">
       <c r="A50" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>27</v>
@@ -3061,7 +3061,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>14</v>
@@ -3070,16 +3070,16 @@
     </row>
     <row r="51" spans="1:11" ht="30">
       <c r="A51" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>27</v>
@@ -3090,10 +3090,10 @@
       <c r="G51" s="1"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K51" s="1"/>
     </row>
@@ -3113,7 +3113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L41"/>
     </sheetView>
   </sheetViews>
@@ -3173,10 +3173,10 @@
     </row>
     <row r="2" spans="1:12" ht="409.5">
       <c r="A2" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>36</v>
@@ -3192,11 +3192,11 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>38</v>
@@ -3204,43 +3204,43 @@
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="75">
       <c r="A4" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>25</v>
@@ -3250,30 +3250,30 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="105">
       <c r="A5" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -3284,27 +3284,27 @@
       <c r="G5" s="1"/>
       <c r="H5" s="10"/>
       <c r="I5" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="75">
       <c r="A6" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>23</v>
@@ -3314,30 +3314,30 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="75">
       <c r="A7" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>23</v>
@@ -3347,97 +3347,97 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="120">
       <c r="A8" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="60">
       <c r="A9" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>14</v>
@@ -3446,16 +3446,16 @@
     </row>
     <row r="11" spans="1:12" ht="105">
       <c r="A11" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
@@ -3466,65 +3466,65 @@
       <c r="G11" s="1"/>
       <c r="H11" s="10"/>
       <c r="I11" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="60">
       <c r="A12" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="45">
       <c r="A13" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>14</v>
@@ -3533,27 +3533,27 @@
     </row>
     <row r="14" spans="1:12" ht="45">
       <c r="A14" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>14</v>
@@ -3562,16 +3562,16 @@
     </row>
     <row r="15" spans="1:12" ht="75">
       <c r="A15" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>1</v>
@@ -3582,500 +3582,500 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="75">
       <c r="A16" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="75">
       <c r="A17" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="75">
       <c r="A18" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="75">
       <c r="A19" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="75">
       <c r="A20" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="195">
       <c r="A21" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="135">
       <c r="A22" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="255">
       <c r="A23" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="135">
       <c r="A24" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="135">
       <c r="A25" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="120">
       <c r="A26" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="120">
       <c r="A27" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="255">
       <c r="A28" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="135">
       <c r="A29" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="120">
       <c r="A30" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="105">
       <c r="A31" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>25</v>
@@ -4085,22 +4085,22 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" ht="60">
       <c r="A32" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>36</v>
@@ -4112,262 +4112,262 @@
         <v>1</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="120">
+    <row r="33" spans="1:11" ht="135">
       <c r="A33" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>225</v>
+        <v>339</v>
       </c>
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" ht="195">
       <c r="A34" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="90">
       <c r="A35" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>28</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" ht="75">
       <c r="A37" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" ht="90">
       <c r="A38" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" ht="60">
       <c r="A39" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:11" ht="45">
       <c r="A40" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>14</v>
@@ -4376,16 +4376,16 @@
     </row>
     <row r="41" spans="1:11" ht="45">
       <c r="A41" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>27</v>
@@ -4396,7 +4396,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>14</v>

</xml_diff>